<commit_message>
updated classification table and legend
</commit_message>
<xml_diff>
--- a/cropScapeDocumentation/CDL_subcategories.xlsx
+++ b/cropScapeDocumentation/CDL_subcategories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leannahouse/Documents/research/imageomics/quest/latLonCover/LatLonCover/cropScapeDocumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{161A444D-E8EA-6A41-9B39-3AA437855E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5EC9C7-F6FA-9943-9AE1-871F2CF3926C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="600" windowWidth="18200" windowHeight="14300" activeTab="2" xr2:uid="{6CA7EC90-0F8F-443F-BB4C-1B27C8F07F03}"/>
+    <workbookView xWindow="2260" yWindow="600" windowWidth="18200" windowHeight="14300" activeTab="4" xr2:uid="{6CA7EC90-0F8F-443F-BB4C-1B27C8F07F03}"/>
   </bookViews>
   <sheets>
     <sheet name="rawList" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="204">
   <si>
     <t>Background</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>Wetland</t>
+  </si>
+  <si>
+    <t>Grassland/Sod grass seed/switchgrass</t>
   </si>
 </sst>
 </file>
@@ -6067,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A553212E-8E5F-2E41-8529-208DA0254E58}">
   <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="C264" sqref="C264"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6926,10 +6929,10 @@
         <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="D61" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -6940,10 +6943,10 @@
         <v>51</v>
       </c>
       <c r="C62" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="D62" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -9683,10 +9686,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCF6703-AD84-1C48-867A-58EFCBB41444}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9736,31 +9739,39 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>150</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C70">
-    <sortCondition ref="A2:A70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C71">
+    <sortCondition ref="A2:A71"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9768,10 +9779,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB310E65-4E75-0349-96C2-85D5F102E027}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9885,49 +9896,57 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>176</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>